<commit_message>
Adição das planilhas das falhas: FSiEOS, FSiVrGMP e FSiVrOS.
</commit_message>
<xml_diff>
--- a/planilhas/deteccao/FAQ/melhores.xlsx
+++ b/planilhas/deteccao/FAQ/melhores.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="EstaPasta_de_trabalho" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="195" windowWidth="19320" windowHeight="12015"/>
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
     <externalReference r:id="rId4"/>
   </externalReferences>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -57,8 +57,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -213,7 +213,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="N8"/>
@@ -231,19 +231,19 @@
             <v>12</v>
           </cell>
           <cell r="C11">
-            <v>4</v>
+            <v>6</v>
           </cell>
           <cell r="D11">
-            <v>23460</v>
+            <v>23976</v>
           </cell>
           <cell r="E11">
-            <v>196.33333333333334</v>
+            <v>0.66666666666666663</v>
           </cell>
           <cell r="F11">
-            <v>343.66666666666669</v>
+            <v>23.333333333333332</v>
           </cell>
           <cell r="G11">
-            <v>540</v>
+            <v>24</v>
           </cell>
         </row>
       </sheetData>
@@ -253,7 +253,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="N14"/>
@@ -274,16 +274,16 @@
             <v>2</v>
           </cell>
           <cell r="D11">
-            <v>23455</v>
+            <v>23979.333333333332</v>
           </cell>
           <cell r="E11">
-            <v>300.33333333333331</v>
+            <v>2.6666666666666665</v>
           </cell>
           <cell r="F11">
-            <v>244.66666666666666</v>
+            <v>18</v>
           </cell>
           <cell r="G11">
-            <v>545</v>
+            <v>20.666666666666668</v>
           </cell>
         </row>
       </sheetData>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink3.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="N20"/>
@@ -308,22 +308,22 @@
       <sheetData sheetId="3">
         <row r="11">
           <cell r="B11">
+            <v>28</v>
+          </cell>
+          <cell r="C11">
+            <v>6</v>
+          </cell>
+          <cell r="D11">
+            <v>23980</v>
+          </cell>
+          <cell r="E11">
+            <v>2.3333333333333335</v>
+          </cell>
+          <cell r="F11">
+            <v>17.666666666666668</v>
+          </cell>
+          <cell r="G11">
             <v>20</v>
-          </cell>
-          <cell r="C11">
-            <v>2</v>
-          </cell>
-          <cell r="D11">
-            <v>23518.666666666668</v>
-          </cell>
-          <cell r="E11">
-            <v>160.33333333333334</v>
-          </cell>
-          <cell r="F11">
-            <v>321</v>
-          </cell>
-          <cell r="G11">
-            <v>481.33333333333337</v>
           </cell>
         </row>
       </sheetData>
@@ -407,6 +407,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -441,6 +442,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -616,7 +618,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Plan4"/>
   <dimension ref="B2:J12"/>
   <sheetViews>
@@ -624,7 +626,7 @@
       <selection activeCell="B2" sqref="B2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="1.42578125" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -634,7 +636,7 @@
     <col min="9" max="9" width="1.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="13" t="s">
         <v>10</v>
       </c>
@@ -645,7 +647,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1">
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -656,7 +658,7 @@
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>8</v>
       </c>
@@ -679,7 +681,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="2:10">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>2</v>
       </c>
@@ -689,30 +691,30 @@
       </c>
       <c r="D6" s="10">
         <f>[1]Melhores!C$11</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E6" s="10">
         <f>[1]Melhores!D$11</f>
-        <v>23460</v>
+        <v>23976</v>
       </c>
       <c r="F6" s="10">
         <f>[1]Melhores!E$11</f>
-        <v>196.33333333333334</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="G6" s="10">
         <f>[1]Melhores!F$11</f>
-        <v>343.66666666666669</v>
+        <v>23.333333333333332</v>
       </c>
       <c r="H6" s="10">
         <f>[1]Melhores!G$11</f>
-        <v>540</v>
+        <v>24</v>
       </c>
       <c r="J6" s="4" t="str">
         <f ca="1">IF(H6=MIN($H$6:$H$8),CELL("lin",H6),"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="2:10">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>3</v>
       </c>
@@ -726,59 +728,59 @@
       </c>
       <c r="E7" s="10">
         <f>[2]Melhores!D$11</f>
-        <v>23455</v>
+        <v>23979.333333333332</v>
       </c>
       <c r="F7" s="10">
         <f>[2]Melhores!E$11</f>
-        <v>300.33333333333331</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="G7" s="10">
         <f>[2]Melhores!F$11</f>
-        <v>244.66666666666666</v>
+        <v>18</v>
       </c>
       <c r="H7" s="10">
         <f>[2]Melhores!G$11</f>
-        <v>545</v>
+        <v>20.666666666666668</v>
       </c>
       <c r="J7" s="4" t="str">
         <f t="shared" ref="J7:J8" ca="1" si="0">IF(H7=MIN($H$6:$H$8),CELL("lin",H7),"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="2:10">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>4</v>
       </c>
       <c r="C8" s="10">
         <f>[3]Melhores!B$11</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D8" s="10">
         <f>[3]Melhores!C$11</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E8" s="10">
         <f>[3]Melhores!D$11</f>
-        <v>23518.666666666668</v>
+        <v>23980</v>
       </c>
       <c r="F8" s="10">
         <f>[3]Melhores!E$11</f>
-        <v>160.33333333333334</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="G8" s="10">
         <f>[3]Melhores!F$11</f>
-        <v>321</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="H8" s="10">
         <f>[3]Melhores!G$11</f>
-        <v>481.33333333333337</v>
+        <v>20</v>
       </c>
       <c r="J8" s="4">
         <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="12" t="s">
         <v>3</v>
       </c>
@@ -789,7 +791,7 @@
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
-    <row r="11" spans="2:10">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -812,34 +814,34 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f ca="1">INDIRECT(CONCATENATE("$B$",SUM($J$6:$J$8)))</f>
         <v>4</v>
       </c>
       <c r="C12" s="3">
         <f ca="1">INDIRECT(CONCATENATE("$C$",SUM($J$6:$J$8)))</f>
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D12" s="3">
         <f ca="1">INDIRECT(CONCATENATE("$D$",SUM($J$6:$J$8)))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E12" s="3">
         <f ca="1">INDIRECT(CONCATENATE("$E$",SUM($J$6:$J$8)))</f>
-        <v>23518.666666666668</v>
+        <v>23980</v>
       </c>
       <c r="F12" s="3">
         <f ca="1">INDIRECT(CONCATENATE("$F$",SUM($J$6:$J$8)))</f>
-        <v>160.33333333333334</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="G12" s="3">
         <f ca="1">INDIRECT(CONCATENATE("$G$",SUM($J$6:$J$8)))</f>
-        <v>321</v>
+        <v>17.666666666666668</v>
       </c>
       <c r="H12" s="3">
         <f ca="1">INDIRECT(CONCATENATE("$H$",SUM($J$6:$J$8)))</f>
-        <v>481.33333333333337</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -851,9 +853,9 @@
   <conditionalFormatting sqref="H6:H8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
-        <cfvo type="min" val="0"/>
+        <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
+        <cfvo type="max"/>
         <color rgb="FF63BE7B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FFF8696B"/>

</xml_diff>